<commit_message>
Gmail report even if Test Failures
</commit_message>
<xml_diff>
--- a/src/main/java/com/konnect/testdata/Groups and Project Creation.xlsx
+++ b/src/main/java/com/konnect/testdata/Groups and Project Creation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="2805" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="2805" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NewGroups" sheetId="1" r:id="rId1"/>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,16 +707,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Merging Sravanthi MyNotes Test
</commit_message>
<xml_diff>
--- a/src/main/java/com/konnect/testdata/Groups and Project Creation.xlsx
+++ b/src/main/java/com/konnect/testdata/Groups and Project Creation.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="2805" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="2805" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewGroups" sheetId="1" r:id="rId1"/>
     <sheet name="KonnectionsUsers" sheetId="9" r:id="rId2"/>
-    <sheet name="Logins" sheetId="10" r:id="rId3"/>
-    <sheet name="ExistingGroups" sheetId="2" r:id="rId4"/>
-    <sheet name="NewProject" sheetId="3" r:id="rId5"/>
-    <sheet name="ProjectLinksCreation" sheetId="7" r:id="rId6"/>
-    <sheet name="ProjectTaskCreation" sheetId="8" r:id="rId7"/>
-    <sheet name="ProjectNotesCreation" sheetId="6" r:id="rId8"/>
+    <sheet name="MyNotesCreation" sheetId="11" r:id="rId3"/>
+    <sheet name="Logins" sheetId="10" r:id="rId4"/>
+    <sheet name="ExistingGroups" sheetId="2" r:id="rId5"/>
+    <sheet name="NewProject" sheetId="3" r:id="rId6"/>
+    <sheet name="ProjectLinksCreation" sheetId="7" r:id="rId7"/>
+    <sheet name="ProjectTaskCreation" sheetId="8" r:id="rId8"/>
+    <sheet name="ProjectNotesCreation" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
   <si>
     <t>Groupname</t>
   </si>
@@ -224,6 +225,36 @@
   </si>
   <si>
     <t>pwd1</t>
+  </si>
+  <si>
+    <t>SourceNote</t>
+  </si>
+  <si>
+    <t>https://gtdataqa.ikonnectplus.com/</t>
+  </si>
+  <si>
+    <t>My Notes</t>
+  </si>
+  <si>
+    <t>Content Portal</t>
+  </si>
+  <si>
+    <t>Konnectplus3</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>ExistingTag</t>
+  </si>
+  <si>
+    <t>CreateNewMyNotesTag</t>
+  </si>
+  <si>
+    <t>Konnectplus33</t>
+  </si>
+  <si>
+    <t>GTKonnect14</t>
   </si>
 </sst>
 </file>
@@ -247,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,6 +376,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -679,7 +720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -725,6 +766,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -760,7 +864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -802,12 +906,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,7 +964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -920,7 +1024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -1051,7 +1155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Merged full code and Added drivers,docuploads folder on 24-04-2018
</commit_message>
<xml_diff>
--- a/src/main/java/com/konnect/testdata/Groups and Project Creation.xlsx
+++ b/src/main/java/com/konnect/testdata/Groups and Project Creation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="2805" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9900" windowHeight="2805" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="NewGroups" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="122">
   <si>
     <t>Groupname</t>
   </si>
@@ -320,9 +320,6 @@
     <t>Newtag</t>
   </si>
   <si>
-    <t>Tags</t>
-  </si>
-  <si>
     <t>Creations of all the links related to konnect portal</t>
   </si>
   <si>
@@ -350,7 +347,55 @@
     <t>Tasks1</t>
   </si>
   <si>
-    <t>GPS test in Konnect Portal1</t>
+    <t>TaskDesc</t>
+  </si>
+  <si>
+    <t>ExistingTags</t>
+  </si>
+  <si>
+    <t>Srcname</t>
+  </si>
+  <si>
+    <t>srcnotes</t>
+  </si>
+  <si>
+    <t>usrnotes</t>
+  </si>
+  <si>
+    <t>NewtaginNotes</t>
+  </si>
+  <si>
+    <t>ExistingTaginNotes</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>NewTaginLinks</t>
+  </si>
+  <si>
+    <t>ExistingTaginLinks</t>
+  </si>
+  <si>
+    <t>FTZ in Konnect Portal</t>
+  </si>
+  <si>
+    <t>ECCN in Tasks</t>
+  </si>
+  <si>
+    <t>ECCN Test</t>
+  </si>
+  <si>
+    <t>Notes in tasks</t>
+  </si>
+  <si>
+    <t>Link to the ECCN</t>
+  </si>
+  <si>
+    <t>Creation of new links against the Task</t>
+  </si>
+  <si>
+    <t>LinksinTasks</t>
   </si>
 </sst>
 </file>
@@ -380,7 +425,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,12 +459,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,7 +536,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1316,19 +1357,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1338,52 +1379,128 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="B1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" s="13" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>